<commit_message>
end of lab 7 session on oct 31
need to get Semaphore_Messages_Processes.c working to pass stuff
</commit_message>
<xml_diff>
--- a/Lab 7 Results.xlsx
+++ b/Lab 7 Results.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Semaphore" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>QNX NODE</t>
   </si>
@@ -64,6 +65,42 @@
   </si>
   <si>
     <t>switch.c</t>
+  </si>
+  <si>
+    <t>time in nano seconds</t>
+  </si>
+  <si>
+    <t>21988528 iterations in 5 seconds</t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>iterations per second</t>
+  </si>
+  <si>
+    <t>MSG Size (bytes)</t>
+  </si>
+  <si>
+    <t>DMA (direct memory access</t>
+  </si>
+  <si>
+    <t>Semaphore Controlled Access</t>
+  </si>
+  <si>
+    <t>Computed Overhead</t>
+  </si>
+  <si>
+    <t>num bytes</t>
+  </si>
+  <si>
+    <t>Semaphore wait time</t>
+  </si>
+  <si>
+    <t>per second</t>
+  </si>
+  <si>
+    <t>nanoseconds</t>
   </si>
 </sst>
 </file>
@@ -130,10 +167,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +454,7 @@
   <dimension ref="A3:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,11 +469,11 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -450,7 +487,7 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -460,8 +497,8 @@
         <f>1/Sheet2!C8</f>
         <v>1.2677690510190836E-7</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -492,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,6 +562,9 @@
       <c r="F7" t="s">
         <v>10</v>
       </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -575,4 +615,292 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f>21988528/5</f>
+        <v>4397705.5999999996</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <f>1235545718/2</f>
+        <v>617772859</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E6" si="0">B4-D4</f>
+        <v>-613375153.39999998</v>
+      </c>
+      <c r="F4">
+        <v>-1127159309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <f>17547190/5</f>
+        <v>3509438</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <f>27453107/2</f>
+        <v>13726553.5</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>-10217115.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>128</v>
+      </c>
+      <c r="B6">
+        <f>10232971/5</f>
+        <v>2046594.2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <f>18977564/5</f>
+        <v>3795512.8</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-1748918.5999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1024</v>
+      </c>
+      <c r="B7">
+        <f>2033944/5</f>
+        <v>406788.8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <f>2209514/5</f>
+        <v>441902.8</v>
+      </c>
+      <c r="E7">
+        <f>B7-D7</f>
+        <v>-35114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:E12" si="1">B4-D10</f>
+        <v>4397705.5999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <f>69623124/5</f>
+        <v>13924624.800000001</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>-10415186.800000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>128</v>
+      </c>
+      <c r="D12">
+        <f>18867288/5</f>
+        <v>3773457.6</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>-1726863.4000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1024</v>
+      </c>
+      <c r="D13">
+        <f>2277124/5</f>
+        <v>455424.8</v>
+      </c>
+      <c r="E13">
+        <f>B7-D13</f>
+        <v>-48636</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <f>1/(D4/1000000000)</f>
+        <v>1.6187179242848544</v>
+      </c>
+      <c r="D18" s="1">
+        <f>1/(B4/1000000000)</f>
+        <v>227.39130150049155</v>
+      </c>
+      <c r="E18" s="1">
+        <f>D18-C18</f>
+        <v>225.7725835762067</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1">
+        <f>1/(D5/1000000000)</f>
+        <v>72.851499103544086</v>
+      </c>
+      <c r="D19" s="1">
+        <f>1/(B5/1000000000)</f>
+        <v>284.94590871814802</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" ref="E19:E21" si="2">D19-C19</f>
+        <v>212.09440961460393</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>128</v>
+      </c>
+      <c r="C20" s="1">
+        <f>1/(D6/1000000000)</f>
+        <v>263.4690100373262</v>
+      </c>
+      <c r="D20" s="1">
+        <f>1/(B6/1000000000)</f>
+        <v>488.61664906506633</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>225.14763902774013</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C21" s="1">
+        <f>1/(D7/1000000000)</f>
+        <v>2262.9410811608345</v>
+      </c>
+      <c r="D21" s="1">
+        <f>1/(B7/1000000000)</f>
+        <v>2458.2781040185964</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="2"/>
+        <v>195.33702285776189</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>4316319</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <f>C29/2</f>
+        <v>2158159.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f>1/C30 *1000000000</f>
+        <v>463.35778240672204</v>
+      </c>
+      <c r="D31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:E17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>